<commit_message>
Updated example data and tableau data results
</commit_message>
<xml_diff>
--- a/data/Portfolio_Activities.xlsx
+++ b/data/Portfolio_Activities.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="17">
   <si>
     <t>anlage</t>
   </si>
@@ -24,6 +24,9 @@
   </si>
   <si>
     <t>volume</t>
+  </si>
+  <si>
+    <t>value</t>
   </si>
   <si>
     <t>fee_buy</t>
@@ -58,15 +61,19 @@
   <si>
     <t>S</t>
   </si>
+  <si>
+    <t>1423.5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="D/M/YYYY"/>
-    <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="165" formatCode="yyyy.m"/>
+    <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="167" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -166,11 +173,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -190,6 +200,9 @@
     <xf borderId="3" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="2" fillId="2" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -197,10 +210,10 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -443,7 +456,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -452,1861 +465,2002 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4">
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="5">
         <v>44803.0</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="6">
         <v>20.0</v>
       </c>
-      <c r="E2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G2" s="3">
+      <c r="E2" s="2">
+        <v>150.0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H2" s="4">
         <v>0.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="5">
+        <v>44803.0</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1300.0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5">
+        <v>44804.0</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0.016</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1310.0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="5">
+        <v>44817.0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1320.0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="5">
+        <v>44819.0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>46.0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>100.0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.005</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0.0164</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0.005</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="5">
+        <v>44838.0</v>
+      </c>
+      <c r="D7" s="11">
+        <v>0.001</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1400.0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="5">
+        <v>44827.0</v>
+      </c>
+      <c r="D8" s="6">
+        <v>25.0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>95.0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.005</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0.0035</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0.005</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="5">
+        <v>44868.0</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.001</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1600.0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="5">
+        <v>44873.0</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0.005</v>
+      </c>
+      <c r="E10" s="2">
+        <v>60000.0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="5">
+        <v>44876.0</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0.09</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1600.0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4">
-        <v>44803.0</v>
-      </c>
-      <c r="D3" s="7">
+      <c r="B12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="5">
+        <v>44900.0</v>
+      </c>
+      <c r="D12" s="6">
+        <v>20.0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>200.0</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0.0059</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0.0036</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0.0059</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="5">
+        <v>44900.0</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0.001</v>
+      </c>
+      <c r="E13" s="2">
+        <v>2000.0</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H13" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="5">
+        <v>44912.0</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0.144</v>
+      </c>
+      <c r="E14" s="2">
+        <v>2100.0</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H14" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="5">
+        <v>44912.0</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0.006</v>
+      </c>
+      <c r="E15" s="2">
+        <v>80000.0</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="5">
+        <v>44929.0</v>
+      </c>
+      <c r="D16" s="6">
+        <v>30.0</v>
+      </c>
+      <c r="E16" s="2">
+        <v>123.0</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="G16" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0.0113</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="5">
+        <v>44930.0</v>
+      </c>
+      <c r="D17" s="6">
+        <v>0.001</v>
+      </c>
+      <c r="E17" s="2">
+        <v>2150.0</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="5">
+        <v>44936.0</v>
+      </c>
+      <c r="D18" s="6">
+        <v>0.001</v>
+      </c>
+      <c r="E18" s="2">
+        <v>2160.0</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="5">
+        <v>44959.0</v>
+      </c>
+      <c r="D19" s="6">
         <v>0.1</v>
       </c>
-      <c r="E3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="s">
+      <c r="E19" s="2">
+        <v>2400.0</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H19" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C20" s="5">
+        <v>44959.0</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.005</v>
+      </c>
+      <c r="E20" s="2">
+        <v>65000.0</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G20" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="5">
+        <v>44970.0</v>
+      </c>
+      <c r="D21" s="6">
+        <v>0.002</v>
+      </c>
+      <c r="E21" s="2">
+        <v>3000.0</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="5">
+        <v>44982.0</v>
+      </c>
+      <c r="D22" s="6">
+        <v>15.0</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G22" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H22" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="5">
+        <v>44986.0</v>
+      </c>
+      <c r="D23" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="E23" s="2">
+        <v>3100.0</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G23" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H23" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="5">
+        <v>44986.0</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0.005</v>
+      </c>
+      <c r="E24" s="2">
+        <v>80000.0</v>
+      </c>
+      <c r="F24" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G24" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H24" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4">
-        <v>44804.0</v>
-      </c>
-      <c r="D4" s="9">
+      <c r="B25" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="13">
+        <v>45168.0</v>
+      </c>
+      <c r="D25" s="6">
+        <v>20.0</v>
+      </c>
+      <c r="E25" s="2">
+        <v>300.0</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G25" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H25" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="13">
+        <v>45168.0</v>
+      </c>
+      <c r="D26" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="E26" s="2">
+        <v>2900.0</v>
+      </c>
+      <c r="F26" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G26" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H26" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="13">
+        <v>45169.0</v>
+      </c>
+      <c r="D27" s="10">
         <v>0.016</v>
       </c>
-      <c r="E4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="6" t="s">
+      <c r="E27" s="2">
+        <v>2900.0</v>
+      </c>
+      <c r="F27" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G27" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H27" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C28" s="13">
+        <v>45182.0</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E28" s="2">
+        <v>2800.0</v>
+      </c>
+      <c r="F28" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G28" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H28" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="13">
+        <v>45184.0</v>
+      </c>
+      <c r="D29" s="4">
+        <v>46.0</v>
+      </c>
+      <c r="E29" s="2">
+        <v>130.0</v>
+      </c>
+      <c r="F29" s="4">
+        <v>0.005</v>
+      </c>
+      <c r="G29" s="4">
+        <v>0.0164</v>
+      </c>
+      <c r="H29" s="4">
+        <v>0.005</v>
+      </c>
+    </row>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="13">
+        <v>45203.0</v>
+      </c>
+      <c r="D30" s="11">
+        <v>0.001</v>
+      </c>
+      <c r="E30" s="2">
+        <v>2800.0</v>
+      </c>
+      <c r="F30" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G30" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H30" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="13">
+        <v>45192.0</v>
+      </c>
+      <c r="D31" s="6">
+        <v>25.0</v>
+      </c>
+      <c r="E31" s="2">
+        <v>180.0</v>
+      </c>
+      <c r="F31" s="4">
+        <v>0.005</v>
+      </c>
+      <c r="G31" s="4">
+        <v>0.0035</v>
+      </c>
+      <c r="H31" s="4">
+        <v>0.005</v>
+      </c>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="13">
+        <v>45233.0</v>
+      </c>
+      <c r="D32" s="6">
+        <v>0.001</v>
+      </c>
+      <c r="E32" s="2">
+        <v>2400.0</v>
+      </c>
+      <c r="F32" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G32" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H32" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="13">
+        <v>45238.0</v>
+      </c>
+      <c r="D33" s="6">
+        <v>0.005</v>
+      </c>
+      <c r="E33" s="2">
+        <v>90000.0</v>
+      </c>
+      <c r="F33" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G33" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H33" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="13">
+        <v>45241.0</v>
+      </c>
+      <c r="D34" s="6">
+        <v>0.09</v>
+      </c>
+      <c r="E34" s="2">
+        <v>3000.0</v>
+      </c>
+      <c r="F34" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G34" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H34" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="A35" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="4">
-        <v>44817.0</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="B35" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="13">
+        <v>45265.0</v>
+      </c>
+      <c r="D35" s="6">
+        <v>20.0</v>
+      </c>
+      <c r="E35" s="2">
+        <v>310.0</v>
+      </c>
+      <c r="F35" s="4">
+        <v>0.0059</v>
+      </c>
+      <c r="G35" s="4">
+        <v>0.0036</v>
+      </c>
+      <c r="H35" s="4">
+        <v>0.0059</v>
+      </c>
+    </row>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="A36" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="13">
+        <v>45265.0</v>
+      </c>
+      <c r="D36" s="6">
+        <v>0.001</v>
+      </c>
+      <c r="E36" s="2">
+        <v>2800.0</v>
+      </c>
+      <c r="F36" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G36" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H36" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="37" ht="15.75" customHeight="1">
+      <c r="A37" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="13">
+        <v>45277.0</v>
+      </c>
+      <c r="D37" s="4">
+        <v>0.144</v>
+      </c>
+      <c r="E37" s="2">
+        <v>2700.0</v>
+      </c>
+      <c r="F37" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G37" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H37" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="A38" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="13">
+        <v>45277.0</v>
+      </c>
+      <c r="D38" s="6">
+        <v>0.006</v>
+      </c>
+      <c r="E38" s="2">
+        <v>67000.0</v>
+      </c>
+      <c r="F38" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G38" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H38" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="39" ht="15.75" customHeight="1">
+      <c r="A39" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="13">
+        <v>45294.0</v>
+      </c>
+      <c r="D39" s="6">
+        <v>30.0</v>
+      </c>
+      <c r="E39" s="2">
+        <v>190.0</v>
+      </c>
+      <c r="F39" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="G39" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H39" s="4">
+        <v>0.0113</v>
+      </c>
+    </row>
+    <row r="40" ht="15.75" customHeight="1">
+      <c r="A40" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="13">
+        <v>45295.0</v>
+      </c>
+      <c r="D40" s="6">
+        <v>0.001</v>
+      </c>
+      <c r="E40" s="2">
+        <v>2500.0</v>
+      </c>
+      <c r="F40" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G40" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H40" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="41" ht="15.75" customHeight="1">
+      <c r="A41" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="13">
+        <v>45301.0</v>
+      </c>
+      <c r="D41" s="6">
+        <v>0.001</v>
+      </c>
+      <c r="E41" s="2">
+        <v>2400.0</v>
+      </c>
+      <c r="F41" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G41" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H41" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="42" ht="15.75" customHeight="1">
+      <c r="A42" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" s="13">
+        <v>45324.0</v>
+      </c>
+      <c r="D42" s="6">
         <v>0.1</v>
       </c>
-      <c r="E5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
+      <c r="E42" s="2">
+        <v>2300.0</v>
+      </c>
+      <c r="F42" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G42" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H42" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="43" ht="15.75" customHeight="1">
+      <c r="A43" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="13">
+        <v>45324.0</v>
+      </c>
+      <c r="D43" s="6">
+        <v>0.005</v>
+      </c>
+      <c r="E43" s="2">
+        <v>75000.0</v>
+      </c>
+      <c r="F43" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G43" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H43" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="44" ht="15.75" customHeight="1">
+      <c r="A44" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="4">
-        <v>44819.0</v>
-      </c>
-      <c r="D6" s="3">
-        <v>46.0</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="B44" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="13">
+        <v>45335.0</v>
+      </c>
+      <c r="D44" s="6">
+        <v>0.002</v>
+      </c>
+      <c r="E44" s="2">
+        <v>2400.0</v>
+      </c>
+      <c r="F44" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G44" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H44" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="45" ht="15.75" customHeight="1">
+      <c r="A45" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" s="13">
+        <v>45347.0</v>
+      </c>
+      <c r="D45" s="6">
+        <v>50.0</v>
+      </c>
+      <c r="E45" s="2">
+        <v>8900.0</v>
+      </c>
+      <c r="F45" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G45" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H45" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="46" ht="15.75" customHeight="1">
+      <c r="A46" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="13">
+        <v>45352.0</v>
+      </c>
+      <c r="D46" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="E46" s="2">
+        <v>2500.0</v>
+      </c>
+      <c r="F46" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G46" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H46" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="47" ht="15.75" customHeight="1">
+      <c r="A47" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="13">
+        <v>45352.0</v>
+      </c>
+      <c r="D47" s="6">
         <v>0.005</v>
       </c>
-      <c r="F6" s="3">
-        <v>0.0164</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0.005</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="4">
-        <v>44838.0</v>
-      </c>
-      <c r="D7" s="10">
-        <v>0.001</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="4">
-        <v>44827.0</v>
-      </c>
-      <c r="D8" s="5">
-        <v>25.0</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0.005</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0.0035</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0.005</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="4">
-        <v>44868.0</v>
-      </c>
-      <c r="D9" s="5">
-        <v>0.001</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="4">
-        <v>44873.0</v>
-      </c>
-      <c r="D10" s="5">
-        <v>0.005</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G10" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="4">
-        <v>44876.0</v>
-      </c>
-      <c r="D11" s="5">
-        <v>0.09</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G11" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="4">
-        <v>44900.0</v>
-      </c>
-      <c r="D12" s="5">
-        <v>20.0</v>
-      </c>
-      <c r="E12" s="3">
-        <v>0.0059</v>
-      </c>
-      <c r="F12" s="3">
-        <v>0.0036</v>
-      </c>
-      <c r="G12" s="3">
-        <v>0.0059</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="4">
-        <v>44900.0</v>
-      </c>
-      <c r="D13" s="5">
-        <v>0.001</v>
-      </c>
-      <c r="E13" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F13" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G13" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="4">
-        <v>44912.0</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0.144</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G14" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="4">
-        <v>44912.0</v>
-      </c>
-      <c r="D15" s="5">
-        <v>0.006</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G15" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="4">
-        <v>44929.0</v>
-      </c>
-      <c r="D16" s="5">
-        <v>30.0</v>
-      </c>
-      <c r="E16" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="F16" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G16" s="3">
-        <v>0.0113</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="4">
-        <v>44930.0</v>
-      </c>
-      <c r="D17" s="5">
-        <v>0.001</v>
-      </c>
-      <c r="E17" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F17" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G17" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="4">
-        <v>44936.0</v>
-      </c>
-      <c r="D18" s="5">
-        <v>0.001</v>
-      </c>
-      <c r="E18" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F18" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G18" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="4">
-        <v>44959.0</v>
-      </c>
-      <c r="D19" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="E19" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F19" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G19" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="4">
-        <v>44959.0</v>
-      </c>
-      <c r="D20" s="5">
-        <v>0.005</v>
-      </c>
-      <c r="E20" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F20" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G20" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="4">
-        <v>44970.0</v>
-      </c>
-      <c r="D21" s="5">
-        <v>0.002</v>
-      </c>
-      <c r="E21" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F21" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G21" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="4">
-        <v>44982.0</v>
-      </c>
-      <c r="D22" s="5">
-        <v>15.0</v>
-      </c>
-      <c r="E22" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F22" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G22" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="4">
-        <v>44986.0</v>
-      </c>
-      <c r="D23" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="E23" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F23" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G23" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="4">
-        <v>44986.0</v>
-      </c>
-      <c r="D24" s="5">
-        <v>0.005</v>
-      </c>
-      <c r="E24" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F24" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G24" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="11">
-        <v>45168.0</v>
-      </c>
-      <c r="D25" s="5">
-        <v>20.0</v>
-      </c>
-      <c r="E25" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F25" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G25" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="11">
-        <v>45168.0</v>
-      </c>
-      <c r="D26" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="E26" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F26" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G26" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="11">
-        <v>45169.0</v>
-      </c>
-      <c r="D27" s="9">
-        <v>0.016</v>
-      </c>
-      <c r="E27" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F27" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G27" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" s="11">
-        <v>45182.0</v>
-      </c>
-      <c r="D28" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="E28" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F28" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G28" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" s="11">
-        <v>45184.0</v>
-      </c>
-      <c r="D29" s="3">
-        <v>46.0</v>
-      </c>
-      <c r="E29" s="3">
-        <v>0.005</v>
-      </c>
-      <c r="F29" s="3">
-        <v>0.0164</v>
-      </c>
-      <c r="G29" s="3">
-        <v>0.005</v>
-      </c>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C30" s="11">
-        <v>45203.0</v>
-      </c>
-      <c r="D30" s="10">
-        <v>0.001</v>
-      </c>
-      <c r="E30" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F30" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G30" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="11">
-        <v>45192.0</v>
-      </c>
-      <c r="D31" s="5">
-        <v>25.0</v>
-      </c>
-      <c r="E31" s="3">
-        <v>0.005</v>
-      </c>
-      <c r="F31" s="3">
-        <v>0.0035</v>
-      </c>
-      <c r="G31" s="3">
-        <v>0.005</v>
-      </c>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="11">
-        <v>45233.0</v>
-      </c>
-      <c r="D32" s="5">
-        <v>0.001</v>
-      </c>
-      <c r="E32" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F32" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G32" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" s="11">
-        <v>45238.0</v>
-      </c>
-      <c r="D33" s="5">
-        <v>0.005</v>
-      </c>
-      <c r="E33" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F33" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G33" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="11">
-        <v>45241.0</v>
-      </c>
-      <c r="D34" s="5">
-        <v>0.09</v>
-      </c>
-      <c r="E34" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F34" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G34" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="11">
-        <v>45265.0</v>
-      </c>
-      <c r="D35" s="5">
-        <v>20.0</v>
-      </c>
-      <c r="E35" s="3">
-        <v>0.0059</v>
-      </c>
-      <c r="F35" s="3">
-        <v>0.0036</v>
-      </c>
-      <c r="G35" s="3">
-        <v>0.0059</v>
-      </c>
-    </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" s="11">
-        <v>45265.0</v>
-      </c>
-      <c r="D36" s="5">
-        <v>0.001</v>
-      </c>
-      <c r="E36" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F36" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G36" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" s="11">
-        <v>45277.0</v>
-      </c>
-      <c r="D37" s="3">
-        <v>0.144</v>
-      </c>
-      <c r="E37" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F37" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G37" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="11">
-        <v>45277.0</v>
-      </c>
-      <c r="D38" s="5">
-        <v>0.006</v>
-      </c>
-      <c r="E38" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F38" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G38" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="11">
-        <v>45294.0</v>
-      </c>
-      <c r="D39" s="5">
-        <v>30.0</v>
-      </c>
-      <c r="E39" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="F39" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G39" s="3">
-        <v>0.0113</v>
-      </c>
-    </row>
-    <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C40" s="11">
-        <v>45295.0</v>
-      </c>
-      <c r="D40" s="5">
-        <v>0.001</v>
-      </c>
-      <c r="E40" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F40" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G40" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C41" s="11">
-        <v>45301.0</v>
-      </c>
-      <c r="D41" s="5">
-        <v>0.001</v>
-      </c>
-      <c r="E41" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F41" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G41" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C42" s="11">
-        <v>45324.0</v>
-      </c>
-      <c r="D42" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="E42" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F42" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G42" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C43" s="11">
-        <v>45324.0</v>
-      </c>
-      <c r="D43" s="5">
-        <v>0.005</v>
-      </c>
-      <c r="E43" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F43" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G43" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C44" s="11">
-        <v>45335.0</v>
-      </c>
-      <c r="D44" s="5">
-        <v>0.002</v>
-      </c>
-      <c r="E44" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F44" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G44" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C45" s="11">
-        <v>45347.0</v>
-      </c>
-      <c r="D45" s="5">
-        <v>50.0</v>
-      </c>
-      <c r="E45" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F45" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G45" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C46" s="11">
-        <v>45352.0</v>
-      </c>
-      <c r="D46" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="E46" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F46" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G46" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C47" s="11">
-        <v>45352.0</v>
-      </c>
-      <c r="D47" s="5">
-        <v>0.005</v>
-      </c>
-      <c r="E47" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F47" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G47" s="3">
+      <c r="E47" s="2">
+        <v>80000.0</v>
+      </c>
+      <c r="F47" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G47" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H47" s="4">
         <v>0.0</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="12"/>
-      <c r="B48" s="12"/>
-      <c r="C48" s="13"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
+      <c r="A48" s="14"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="12"/>
-      <c r="B49" s="12"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="12"/>
-      <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
+      <c r="A49" s="14"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="12"/>
-      <c r="B50" s="12"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
-      <c r="G50" s="12"/>
+      <c r="A50" s="14"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="12"/>
-      <c r="B51" s="12"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
+      <c r="A51" s="14"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="12"/>
-      <c r="B52" s="12"/>
-      <c r="C52" s="13"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
-      <c r="F52" s="12"/>
-      <c r="G52" s="12"/>
+      <c r="A52" s="14"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="12"/>
-      <c r="B53" s="12"/>
-      <c r="C53" s="13"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="12"/>
+      <c r="A53" s="14"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="12"/>
-      <c r="B54" s="12"/>
-      <c r="C54" s="13"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="12"/>
+      <c r="A54" s="14"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="12"/>
-      <c r="B55" s="12"/>
-      <c r="C55" s="13"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
-      <c r="G55" s="12"/>
+      <c r="A55" s="14"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="12"/>
-      <c r="B56" s="12"/>
-      <c r="C56" s="13"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
-      <c r="G56" s="12"/>
+      <c r="A56" s="14"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="12"/>
-      <c r="B57" s="12"/>
-      <c r="C57" s="13"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="12"/>
-      <c r="F57" s="12"/>
-      <c r="G57" s="12"/>
+      <c r="A57" s="14"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="14"/>
+      <c r="H57" s="14"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="12"/>
-      <c r="B58" s="12"/>
-      <c r="C58" s="13"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="12"/>
-      <c r="F58" s="12"/>
-      <c r="G58" s="12"/>
+      <c r="A58" s="14"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="12"/>
-      <c r="B59" s="12"/>
-      <c r="C59" s="13"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
-      <c r="G59" s="12"/>
+      <c r="A59" s="14"/>
+      <c r="B59" s="14"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="14"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="12"/>
-      <c r="B60" s="12"/>
-      <c r="C60" s="13"/>
-      <c r="D60" s="12"/>
-      <c r="E60" s="12"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="12"/>
+      <c r="A60" s="14"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="14"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="14"/>
+      <c r="H60" s="14"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="12"/>
-      <c r="B61" s="12"/>
-      <c r="C61" s="13"/>
-      <c r="D61" s="12"/>
-      <c r="E61" s="12"/>
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
+      <c r="A61" s="14"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="14"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="14"/>
+      <c r="H61" s="14"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="12"/>
-      <c r="B62" s="12"/>
-      <c r="C62" s="13"/>
-      <c r="E62" s="12"/>
-      <c r="F62" s="12"/>
-      <c r="G62" s="12"/>
+      <c r="A62" s="14"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="15"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="14"/>
+      <c r="H62" s="14"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="12"/>
-      <c r="B63" s="12"/>
-      <c r="C63" s="13"/>
-      <c r="E63" s="12"/>
-      <c r="F63" s="12"/>
-      <c r="G63" s="12"/>
+      <c r="A63" s="14"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="15"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="14"/>
+      <c r="H63" s="14"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="12"/>
-      <c r="B64" s="12"/>
-      <c r="C64" s="13"/>
-      <c r="E64" s="12"/>
-      <c r="F64" s="12"/>
-      <c r="G64" s="12"/>
+      <c r="A64" s="14"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="15"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="14"/>
+      <c r="H64" s="14"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="12"/>
-      <c r="B65" s="12"/>
-      <c r="C65" s="13"/>
-      <c r="E65" s="12"/>
-      <c r="F65" s="12"/>
-      <c r="G65" s="12"/>
+      <c r="A65" s="14"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="15"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="12"/>
-      <c r="B66" s="12"/>
-      <c r="C66" s="13"/>
-      <c r="E66" s="12"/>
-      <c r="F66" s="12"/>
-      <c r="G66" s="12"/>
+      <c r="A66" s="14"/>
+      <c r="B66" s="14"/>
+      <c r="C66" s="15"/>
+      <c r="F66" s="14"/>
+      <c r="G66" s="14"/>
+      <c r="H66" s="14"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="12"/>
-      <c r="B67" s="12"/>
-      <c r="C67" s="13"/>
-      <c r="E67" s="12"/>
-      <c r="F67" s="12"/>
-      <c r="G67" s="12"/>
+      <c r="A67" s="14"/>
+      <c r="B67" s="14"/>
+      <c r="C67" s="15"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="14"/>
+      <c r="H67" s="14"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="12"/>
-      <c r="B68" s="12"/>
-      <c r="C68" s="13"/>
-      <c r="E68" s="12"/>
-      <c r="F68" s="12"/>
-      <c r="G68" s="12"/>
+      <c r="A68" s="14"/>
+      <c r="B68" s="14"/>
+      <c r="C68" s="15"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="14"/>
+      <c r="H68" s="14"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="12"/>
-      <c r="B69" s="12"/>
-      <c r="C69" s="13"/>
-      <c r="E69" s="12"/>
-      <c r="F69" s="12"/>
-      <c r="G69" s="12"/>
+      <c r="A69" s="14"/>
+      <c r="B69" s="14"/>
+      <c r="C69" s="15"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="14"/>
+      <c r="H69" s="14"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="12"/>
-      <c r="B70" s="12"/>
-      <c r="C70" s="13"/>
-      <c r="E70" s="12"/>
-      <c r="F70" s="12"/>
-      <c r="G70" s="12"/>
+      <c r="A70" s="14"/>
+      <c r="B70" s="14"/>
+      <c r="C70" s="15"/>
+      <c r="F70" s="14"/>
+      <c r="G70" s="14"/>
+      <c r="H70" s="14"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="12"/>
-      <c r="B71" s="12"/>
-      <c r="C71" s="13"/>
-      <c r="E71" s="12"/>
-      <c r="F71" s="12"/>
+      <c r="A71" s="14"/>
+      <c r="B71" s="14"/>
+      <c r="C71" s="15"/>
+      <c r="F71" s="14"/>
+      <c r="G71" s="14"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="12"/>
-      <c r="B72" s="12"/>
-      <c r="C72" s="13"/>
-      <c r="E72" s="12"/>
-      <c r="F72" s="12"/>
-      <c r="G72" s="12"/>
+      <c r="A72" s="14"/>
+      <c r="B72" s="14"/>
+      <c r="C72" s="15"/>
+      <c r="F72" s="14"/>
+      <c r="G72" s="14"/>
+      <c r="H72" s="14"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="12"/>
-      <c r="B73" s="12"/>
-      <c r="C73" s="13"/>
-      <c r="E73" s="12"/>
-      <c r="F73" s="12"/>
-      <c r="G73" s="12"/>
+      <c r="A73" s="14"/>
+      <c r="B73" s="14"/>
+      <c r="C73" s="15"/>
+      <c r="F73" s="14"/>
+      <c r="G73" s="14"/>
+      <c r="H73" s="14"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="12"/>
-      <c r="B74" s="12"/>
-      <c r="C74" s="13"/>
-      <c r="E74" s="12"/>
-      <c r="F74" s="12"/>
-      <c r="G74" s="12"/>
+      <c r="A74" s="14"/>
+      <c r="B74" s="14"/>
+      <c r="C74" s="15"/>
+      <c r="F74" s="14"/>
+      <c r="G74" s="14"/>
+      <c r="H74" s="14"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="12"/>
-      <c r="B75" s="12"/>
-      <c r="C75" s="13"/>
-      <c r="E75" s="12"/>
-      <c r="F75" s="12"/>
-      <c r="G75" s="12"/>
+      <c r="A75" s="14"/>
+      <c r="B75" s="14"/>
+      <c r="C75" s="15"/>
+      <c r="F75" s="14"/>
+      <c r="G75" s="14"/>
+      <c r="H75" s="14"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="12"/>
-      <c r="B76" s="12"/>
-      <c r="C76" s="13"/>
-      <c r="E76" s="12"/>
-      <c r="F76" s="12"/>
-      <c r="G76" s="12"/>
+      <c r="A76" s="14"/>
+      <c r="B76" s="14"/>
+      <c r="C76" s="15"/>
+      <c r="F76" s="14"/>
+      <c r="G76" s="14"/>
+      <c r="H76" s="14"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="12"/>
-      <c r="B77" s="12"/>
-      <c r="C77" s="13"/>
-      <c r="E77" s="12"/>
-      <c r="F77" s="12"/>
-      <c r="G77" s="12"/>
+      <c r="A77" s="14"/>
+      <c r="B77" s="14"/>
+      <c r="C77" s="15"/>
+      <c r="F77" s="14"/>
+      <c r="G77" s="14"/>
+      <c r="H77" s="14"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="12"/>
-      <c r="B78" s="12"/>
-      <c r="C78" s="13"/>
-      <c r="E78" s="12"/>
-      <c r="F78" s="12"/>
-      <c r="G78" s="12"/>
+      <c r="A78" s="14"/>
+      <c r="B78" s="14"/>
+      <c r="C78" s="15"/>
+      <c r="F78" s="14"/>
+      <c r="G78" s="14"/>
+      <c r="H78" s="14"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="12"/>
-      <c r="B79" s="12"/>
-      <c r="C79" s="13"/>
-      <c r="E79" s="12"/>
-      <c r="F79" s="12"/>
-      <c r="G79" s="12"/>
+      <c r="A79" s="14"/>
+      <c r="B79" s="14"/>
+      <c r="C79" s="15"/>
+      <c r="F79" s="14"/>
+      <c r="G79" s="14"/>
+      <c r="H79" s="14"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="12"/>
-      <c r="B80" s="12"/>
-      <c r="C80" s="13"/>
-      <c r="D80" s="12"/>
-      <c r="E80" s="12"/>
-      <c r="F80" s="12"/>
-      <c r="G80" s="12"/>
+      <c r="A80" s="14"/>
+      <c r="B80" s="14"/>
+      <c r="C80" s="15"/>
+      <c r="D80" s="14"/>
+      <c r="F80" s="14"/>
+      <c r="G80" s="14"/>
+      <c r="H80" s="14"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="12"/>
-      <c r="B81" s="12"/>
-      <c r="C81" s="13"/>
-      <c r="E81" s="12"/>
-      <c r="F81" s="12"/>
-      <c r="G81" s="12"/>
+      <c r="A81" s="14"/>
+      <c r="B81" s="14"/>
+      <c r="C81" s="15"/>
+      <c r="F81" s="14"/>
+      <c r="G81" s="14"/>
+      <c r="H81" s="14"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="12"/>
-      <c r="B82" s="12"/>
-      <c r="C82" s="13"/>
-      <c r="E82" s="12"/>
-      <c r="F82" s="12"/>
-      <c r="G82" s="12"/>
+      <c r="A82" s="14"/>
+      <c r="B82" s="14"/>
+      <c r="C82" s="15"/>
+      <c r="F82" s="14"/>
+      <c r="G82" s="14"/>
+      <c r="H82" s="14"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="12"/>
-      <c r="B83" s="12"/>
-      <c r="C83" s="13"/>
-      <c r="D83" s="12"/>
-      <c r="E83" s="12"/>
-      <c r="F83" s="12"/>
-      <c r="G83" s="12"/>
+      <c r="A83" s="14"/>
+      <c r="B83" s="14"/>
+      <c r="C83" s="15"/>
+      <c r="D83" s="14"/>
+      <c r="F83" s="14"/>
+      <c r="G83" s="14"/>
+      <c r="H83" s="14"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="12"/>
-      <c r="B84" s="12"/>
-      <c r="C84" s="13"/>
-      <c r="D84" s="12"/>
-      <c r="E84" s="12"/>
-      <c r="F84" s="12"/>
-      <c r="G84" s="12"/>
+      <c r="A84" s="14"/>
+      <c r="B84" s="14"/>
+      <c r="C84" s="15"/>
+      <c r="D84" s="14"/>
+      <c r="F84" s="14"/>
+      <c r="G84" s="14"/>
+      <c r="H84" s="14"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="12"/>
-      <c r="B85" s="12"/>
-      <c r="C85" s="13"/>
-      <c r="E85" s="12"/>
-      <c r="F85" s="12"/>
-      <c r="G85" s="12"/>
+      <c r="A85" s="14"/>
+      <c r="B85" s="14"/>
+      <c r="C85" s="15"/>
+      <c r="F85" s="14"/>
+      <c r="G85" s="14"/>
+      <c r="H85" s="14"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="12"/>
-      <c r="B86" s="12"/>
-      <c r="C86" s="13"/>
-      <c r="E86" s="12"/>
-      <c r="F86" s="12"/>
-      <c r="G86" s="12"/>
+      <c r="A86" s="14"/>
+      <c r="B86" s="14"/>
+      <c r="C86" s="15"/>
+      <c r="F86" s="14"/>
+      <c r="G86" s="14"/>
+      <c r="H86" s="14"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="12"/>
-      <c r="B87" s="12"/>
-      <c r="C87" s="13"/>
-      <c r="E87" s="12"/>
-      <c r="F87" s="12"/>
-      <c r="G87" s="12"/>
+      <c r="A87" s="14"/>
+      <c r="B87" s="14"/>
+      <c r="C87" s="15"/>
+      <c r="F87" s="14"/>
+      <c r="G87" s="14"/>
+      <c r="H87" s="14"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="12"/>
-      <c r="B88" s="12"/>
-      <c r="C88" s="13"/>
-      <c r="E88" s="12"/>
-      <c r="F88" s="12"/>
-      <c r="G88" s="12"/>
+      <c r="A88" s="14"/>
+      <c r="B88" s="14"/>
+      <c r="C88" s="15"/>
+      <c r="F88" s="14"/>
+      <c r="G88" s="14"/>
+      <c r="H88" s="14"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="12"/>
-      <c r="B89" s="12"/>
-      <c r="C89" s="13"/>
-      <c r="D89" s="12"/>
-      <c r="E89" s="12"/>
-      <c r="F89" s="12"/>
-      <c r="G89" s="12"/>
+      <c r="A89" s="14"/>
+      <c r="B89" s="14"/>
+      <c r="C89" s="15"/>
+      <c r="D89" s="14"/>
+      <c r="F89" s="14"/>
+      <c r="G89" s="14"/>
+      <c r="H89" s="14"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="12"/>
-      <c r="B90" s="12"/>
-      <c r="C90" s="13"/>
-      <c r="D90" s="12"/>
-      <c r="E90" s="12"/>
-      <c r="F90" s="12"/>
-      <c r="G90" s="12"/>
+      <c r="A90" s="14"/>
+      <c r="B90" s="14"/>
+      <c r="C90" s="15"/>
+      <c r="D90" s="14"/>
+      <c r="F90" s="14"/>
+      <c r="G90" s="14"/>
+      <c r="H90" s="14"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="12"/>
-      <c r="B91" s="12"/>
-      <c r="C91" s="13"/>
-      <c r="E91" s="12"/>
-      <c r="F91" s="12"/>
-      <c r="G91" s="12"/>
+      <c r="A91" s="14"/>
+      <c r="B91" s="14"/>
+      <c r="C91" s="15"/>
+      <c r="F91" s="14"/>
+      <c r="G91" s="14"/>
+      <c r="H91" s="14"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="12"/>
-      <c r="B92" s="12"/>
-      <c r="C92" s="13"/>
-      <c r="E92" s="12"/>
-      <c r="F92" s="12"/>
-      <c r="G92" s="12"/>
+      <c r="A92" s="14"/>
+      <c r="B92" s="14"/>
+      <c r="C92" s="15"/>
+      <c r="F92" s="14"/>
+      <c r="G92" s="14"/>
+      <c r="H92" s="14"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="12"/>
-      <c r="B93" s="12"/>
-      <c r="C93" s="13"/>
-      <c r="E93" s="12"/>
-      <c r="F93" s="12"/>
-      <c r="G93" s="12"/>
+      <c r="A93" s="14"/>
+      <c r="B93" s="14"/>
+      <c r="C93" s="15"/>
+      <c r="F93" s="14"/>
+      <c r="G93" s="14"/>
+      <c r="H93" s="14"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="12"/>
-      <c r="B94" s="12"/>
-      <c r="C94" s="13"/>
-      <c r="D94" s="12"/>
-      <c r="E94" s="12"/>
-      <c r="F94" s="12"/>
-      <c r="G94" s="12"/>
+      <c r="A94" s="14"/>
+      <c r="B94" s="14"/>
+      <c r="C94" s="15"/>
+      <c r="D94" s="14"/>
+      <c r="F94" s="14"/>
+      <c r="G94" s="14"/>
+      <c r="H94" s="14"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="12"/>
-      <c r="B95" s="12"/>
-      <c r="C95" s="13"/>
-      <c r="E95" s="12"/>
-      <c r="F95" s="12"/>
-      <c r="G95" s="12"/>
+      <c r="A95" s="14"/>
+      <c r="B95" s="14"/>
+      <c r="C95" s="15"/>
+      <c r="F95" s="14"/>
+      <c r="G95" s="14"/>
+      <c r="H95" s="14"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="A96" s="12"/>
-      <c r="B96" s="12"/>
-      <c r="C96" s="13"/>
-      <c r="E96" s="12"/>
-      <c r="F96" s="12"/>
-      <c r="G96" s="12"/>
+      <c r="A96" s="14"/>
+      <c r="B96" s="14"/>
+      <c r="C96" s="15"/>
+      <c r="F96" s="14"/>
+      <c r="G96" s="14"/>
+      <c r="H96" s="14"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="A97" s="12"/>
-      <c r="B97" s="12"/>
-      <c r="C97" s="13"/>
-      <c r="E97" s="12"/>
-      <c r="F97" s="12"/>
-      <c r="G97" s="12"/>
+      <c r="A97" s="14"/>
+      <c r="B97" s="14"/>
+      <c r="C97" s="15"/>
+      <c r="F97" s="14"/>
+      <c r="G97" s="14"/>
+      <c r="H97" s="14"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="A98" s="12"/>
-      <c r="B98" s="12"/>
-      <c r="C98" s="13"/>
-      <c r="E98" s="12"/>
-      <c r="F98" s="12"/>
-      <c r="G98" s="12"/>
+      <c r="A98" s="14"/>
+      <c r="B98" s="14"/>
+      <c r="C98" s="15"/>
+      <c r="F98" s="14"/>
+      <c r="G98" s="14"/>
+      <c r="H98" s="14"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="A99" s="12"/>
-      <c r="B99" s="12"/>
-      <c r="C99" s="13"/>
-      <c r="D99" s="12"/>
-      <c r="E99" s="12"/>
-      <c r="F99" s="12"/>
-      <c r="G99" s="12"/>
+      <c r="A99" s="14"/>
+      <c r="B99" s="14"/>
+      <c r="C99" s="15"/>
+      <c r="D99" s="14"/>
+      <c r="F99" s="14"/>
+      <c r="G99" s="14"/>
+      <c r="H99" s="14"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="A100" s="12"/>
-      <c r="B100" s="12"/>
-      <c r="C100" s="13"/>
-      <c r="E100" s="12"/>
-      <c r="F100" s="12"/>
-      <c r="G100" s="12"/>
+      <c r="A100" s="14"/>
+      <c r="B100" s="14"/>
+      <c r="C100" s="15"/>
+      <c r="F100" s="14"/>
+      <c r="G100" s="14"/>
+      <c r="H100" s="14"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="A101" s="12"/>
-      <c r="B101" s="12"/>
-      <c r="C101" s="13"/>
-      <c r="E101" s="12"/>
-      <c r="F101" s="12"/>
-      <c r="G101" s="12"/>
+      <c r="A101" s="14"/>
+      <c r="B101" s="14"/>
+      <c r="C101" s="15"/>
+      <c r="F101" s="14"/>
+      <c r="G101" s="14"/>
+      <c r="H101" s="14"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="A102" s="12"/>
-      <c r="B102" s="12"/>
-      <c r="C102" s="13"/>
-      <c r="E102" s="12"/>
-      <c r="F102" s="12"/>
-      <c r="G102" s="12"/>
+      <c r="A102" s="14"/>
+      <c r="B102" s="14"/>
+      <c r="C102" s="15"/>
+      <c r="F102" s="14"/>
+      <c r="G102" s="14"/>
+      <c r="H102" s="14"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="A103" s="12"/>
-      <c r="B103" s="12"/>
-      <c r="C103" s="13"/>
-      <c r="E103" s="12"/>
-      <c r="F103" s="12"/>
-      <c r="G103" s="12"/>
+      <c r="A103" s="14"/>
+      <c r="B103" s="14"/>
+      <c r="C103" s="15"/>
+      <c r="F103" s="14"/>
+      <c r="G103" s="14"/>
+      <c r="H103" s="14"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="A104" s="12"/>
-      <c r="B104" s="12"/>
-      <c r="C104" s="13"/>
-      <c r="E104" s="12"/>
-      <c r="F104" s="12"/>
-      <c r="G104" s="12"/>
+      <c r="A104" s="14"/>
+      <c r="B104" s="14"/>
+      <c r="C104" s="15"/>
+      <c r="F104" s="14"/>
+      <c r="G104" s="14"/>
+      <c r="H104" s="14"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="A105" s="12"/>
-      <c r="B105" s="12"/>
-      <c r="C105" s="13"/>
-      <c r="E105" s="12"/>
-      <c r="F105" s="12"/>
-      <c r="G105" s="12"/>
+      <c r="A105" s="14"/>
+      <c r="B105" s="14"/>
+      <c r="C105" s="15"/>
+      <c r="F105" s="14"/>
+      <c r="G105" s="14"/>
+      <c r="H105" s="14"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="A106" s="12"/>
-      <c r="B106" s="12"/>
-      <c r="C106" s="13"/>
-      <c r="E106" s="12"/>
-      <c r="F106" s="12"/>
-      <c r="G106" s="12"/>
+      <c r="A106" s="14"/>
+      <c r="B106" s="14"/>
+      <c r="C106" s="15"/>
+      <c r="F106" s="14"/>
+      <c r="G106" s="14"/>
+      <c r="H106" s="14"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="A107" s="12"/>
-      <c r="B107" s="12"/>
-      <c r="C107" s="13"/>
-      <c r="E107" s="12"/>
-      <c r="F107" s="12"/>
-      <c r="G107" s="12"/>
+      <c r="A107" s="14"/>
+      <c r="B107" s="14"/>
+      <c r="C107" s="15"/>
+      <c r="F107" s="14"/>
+      <c r="G107" s="14"/>
+      <c r="H107" s="14"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="A108" s="12"/>
-      <c r="B108" s="12"/>
-      <c r="C108" s="13"/>
-      <c r="E108" s="12"/>
-      <c r="F108" s="12"/>
-      <c r="G108" s="12"/>
+      <c r="A108" s="14"/>
+      <c r="B108" s="14"/>
+      <c r="C108" s="15"/>
+      <c r="F108" s="14"/>
+      <c r="G108" s="14"/>
+      <c r="H108" s="14"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="A109" s="12"/>
-      <c r="B109" s="12"/>
-      <c r="C109" s="13"/>
-      <c r="E109" s="12"/>
-      <c r="F109" s="12"/>
-      <c r="G109" s="12"/>
+      <c r="A109" s="14"/>
+      <c r="B109" s="14"/>
+      <c r="C109" s="15"/>
+      <c r="F109" s="14"/>
+      <c r="G109" s="14"/>
+      <c r="H109" s="14"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="A110" s="12"/>
-      <c r="B110" s="12"/>
-      <c r="C110" s="13"/>
-      <c r="E110" s="12"/>
-      <c r="F110" s="12"/>
-      <c r="G110" s="12"/>
+      <c r="A110" s="14"/>
+      <c r="B110" s="14"/>
+      <c r="C110" s="15"/>
+      <c r="F110" s="14"/>
+      <c r="G110" s="14"/>
+      <c r="H110" s="14"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="A111" s="12"/>
-      <c r="B111" s="12"/>
-      <c r="C111" s="13"/>
-      <c r="E111" s="12"/>
-      <c r="F111" s="12"/>
-      <c r="G111" s="12"/>
+      <c r="A111" s="14"/>
+      <c r="B111" s="14"/>
+      <c r="C111" s="15"/>
+      <c r="F111" s="14"/>
+      <c r="G111" s="14"/>
+      <c r="H111" s="14"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="A112" s="12"/>
-      <c r="B112" s="12"/>
-      <c r="C112" s="13"/>
-      <c r="E112" s="12"/>
-      <c r="F112" s="12"/>
-      <c r="G112" s="12"/>
+      <c r="A112" s="14"/>
+      <c r="B112" s="14"/>
+      <c r="C112" s="15"/>
+      <c r="F112" s="14"/>
+      <c r="G112" s="14"/>
+      <c r="H112" s="14"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="A113" s="12"/>
-      <c r="B113" s="12"/>
-      <c r="C113" s="13"/>
-      <c r="E113" s="12"/>
-      <c r="F113" s="12"/>
-      <c r="G113" s="12"/>
+      <c r="A113" s="14"/>
+      <c r="B113" s="14"/>
+      <c r="C113" s="15"/>
+      <c r="F113" s="14"/>
+      <c r="G113" s="14"/>
+      <c r="H113" s="14"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="A114" s="12"/>
-      <c r="B114" s="12"/>
-      <c r="C114" s="13"/>
-      <c r="E114" s="12"/>
-      <c r="F114" s="12"/>
-      <c r="G114" s="12"/>
+      <c r="A114" s="14"/>
+      <c r="B114" s="14"/>
+      <c r="C114" s="15"/>
+      <c r="F114" s="14"/>
+      <c r="G114" s="14"/>
+      <c r="H114" s="14"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="A115" s="12"/>
-      <c r="B115" s="12"/>
-      <c r="C115" s="13"/>
-      <c r="E115" s="12"/>
-      <c r="F115" s="12"/>
-      <c r="G115" s="12"/>
+      <c r="A115" s="14"/>
+      <c r="B115" s="14"/>
+      <c r="C115" s="15"/>
+      <c r="F115" s="14"/>
+      <c r="G115" s="14"/>
+      <c r="H115" s="14"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="A116" s="12"/>
-      <c r="B116" s="12"/>
-      <c r="C116" s="13"/>
-      <c r="E116" s="12"/>
-      <c r="F116" s="12"/>
-      <c r="G116" s="12"/>
+      <c r="A116" s="14"/>
+      <c r="B116" s="14"/>
+      <c r="C116" s="15"/>
+      <c r="F116" s="14"/>
+      <c r="G116" s="14"/>
+      <c r="H116" s="14"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="A117" s="12"/>
-      <c r="B117" s="12"/>
-      <c r="C117" s="13"/>
-      <c r="E117" s="12"/>
-      <c r="F117" s="12"/>
-      <c r="G117" s="12"/>
+      <c r="A117" s="14"/>
+      <c r="B117" s="14"/>
+      <c r="C117" s="15"/>
+      <c r="F117" s="14"/>
+      <c r="G117" s="14"/>
+      <c r="H117" s="14"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="A118" s="12"/>
-      <c r="B118" s="12"/>
-      <c r="C118" s="13"/>
-      <c r="E118" s="12"/>
-      <c r="F118" s="12"/>
-      <c r="G118" s="12"/>
+      <c r="A118" s="14"/>
+      <c r="B118" s="14"/>
+      <c r="C118" s="15"/>
+      <c r="F118" s="14"/>
+      <c r="G118" s="14"/>
+      <c r="H118" s="14"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="A119" s="12"/>
-      <c r="B119" s="12"/>
-      <c r="C119" s="13"/>
-      <c r="E119" s="12"/>
-      <c r="F119" s="12"/>
-      <c r="G119" s="12"/>
+      <c r="A119" s="14"/>
+      <c r="B119" s="14"/>
+      <c r="C119" s="15"/>
+      <c r="F119" s="14"/>
+      <c r="G119" s="14"/>
+      <c r="H119" s="14"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="A120" s="12"/>
-      <c r="B120" s="12"/>
-      <c r="C120" s="13"/>
-      <c r="E120" s="12"/>
-      <c r="F120" s="12"/>
-      <c r="G120" s="12"/>
+      <c r="A120" s="14"/>
+      <c r="B120" s="14"/>
+      <c r="C120" s="15"/>
+      <c r="F120" s="14"/>
+      <c r="G120" s="14"/>
+      <c r="H120" s="14"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="A121" s="12"/>
-      <c r="B121" s="12"/>
-      <c r="C121" s="13"/>
-      <c r="E121" s="12"/>
-      <c r="F121" s="12"/>
-      <c r="G121" s="12"/>
+      <c r="A121" s="14"/>
+      <c r="B121" s="14"/>
+      <c r="C121" s="15"/>
+      <c r="F121" s="14"/>
+      <c r="G121" s="14"/>
+      <c r="H121" s="14"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="A122" s="12"/>
-      <c r="B122" s="12"/>
-      <c r="C122" s="13"/>
-      <c r="E122" s="12"/>
-      <c r="F122" s="12"/>
-      <c r="G122" s="12"/>
+      <c r="A122" s="14"/>
+      <c r="B122" s="14"/>
+      <c r="C122" s="15"/>
+      <c r="F122" s="14"/>
+      <c r="G122" s="14"/>
+      <c r="H122" s="14"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="A123" s="12"/>
-      <c r="B123" s="12"/>
-      <c r="C123" s="13"/>
-      <c r="E123" s="12"/>
-      <c r="F123" s="12"/>
-      <c r="G123" s="12"/>
+      <c r="A123" s="14"/>
+      <c r="B123" s="14"/>
+      <c r="C123" s="15"/>
+      <c r="F123" s="14"/>
+      <c r="G123" s="14"/>
+      <c r="H123" s="14"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="A124" s="12"/>
-      <c r="B124" s="12"/>
-      <c r="C124" s="13"/>
-      <c r="E124" s="12"/>
-      <c r="F124" s="12"/>
-      <c r="G124" s="12"/>
+      <c r="A124" s="14"/>
+      <c r="B124" s="14"/>
+      <c r="C124" s="15"/>
+      <c r="F124" s="14"/>
+      <c r="G124" s="14"/>
+      <c r="H124" s="14"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="A125" s="12"/>
-      <c r="B125" s="12"/>
-      <c r="C125" s="13"/>
-      <c r="E125" s="12"/>
-      <c r="F125" s="12"/>
-      <c r="G125" s="12"/>
+      <c r="A125" s="14"/>
+      <c r="B125" s="14"/>
+      <c r="C125" s="15"/>
+      <c r="F125" s="14"/>
+      <c r="G125" s="14"/>
+      <c r="H125" s="14"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="A126" s="14"/>
-      <c r="B126" s="14"/>
-      <c r="C126" s="15"/>
-      <c r="E126" s="14"/>
-      <c r="F126" s="14"/>
-      <c r="G126" s="14"/>
+      <c r="A126" s="16"/>
+      <c r="B126" s="16"/>
+      <c r="C126" s="17"/>
+      <c r="F126" s="16"/>
+      <c r="G126" s="16"/>
+      <c r="H126" s="16"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="A127" s="14"/>
-      <c r="B127" s="14"/>
-      <c r="C127" s="15"/>
-      <c r="E127" s="14"/>
-      <c r="F127" s="14"/>
-      <c r="G127" s="14"/>
+      <c r="A127" s="16"/>
+      <c r="B127" s="16"/>
+      <c r="C127" s="17"/>
+      <c r="F127" s="16"/>
+      <c r="G127" s="16"/>
+      <c r="H127" s="16"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="A128" s="14"/>
-      <c r="B128" s="14"/>
-      <c r="C128" s="15"/>
-      <c r="E128" s="14"/>
-      <c r="F128" s="14"/>
-      <c r="G128" s="14"/>
+      <c r="A128" s="16"/>
+      <c r="B128" s="16"/>
+      <c r="C128" s="17"/>
+      <c r="F128" s="16"/>
+      <c r="G128" s="16"/>
+      <c r="H128" s="16"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="A129" s="14"/>
-      <c r="B129" s="14"/>
-      <c r="C129" s="15"/>
-      <c r="E129" s="14"/>
-      <c r="F129" s="14"/>
-      <c r="G129" s="14"/>
+      <c r="A129" s="16"/>
+      <c r="B129" s="16"/>
+      <c r="C129" s="17"/>
+      <c r="F129" s="16"/>
+      <c r="G129" s="16"/>
+      <c r="H129" s="16"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="A130" s="14"/>
-      <c r="B130" s="14"/>
-      <c r="C130" s="15"/>
-      <c r="E130" s="14"/>
-      <c r="F130" s="14"/>
-      <c r="G130" s="14"/>
+      <c r="A130" s="16"/>
+      <c r="B130" s="16"/>
+      <c r="C130" s="17"/>
+      <c r="F130" s="16"/>
+      <c r="G130" s="16"/>
+      <c r="H130" s="16"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="A131" s="14"/>
-      <c r="B131" s="14"/>
-      <c r="C131" s="15"/>
-      <c r="E131" s="14"/>
-      <c r="F131" s="14"/>
-      <c r="G131" s="14"/>
+      <c r="A131" s="16"/>
+      <c r="B131" s="16"/>
+      <c r="C131" s="17"/>
+      <c r="F131" s="16"/>
+      <c r="G131" s="16"/>
+      <c r="H131" s="16"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="A132" s="14"/>
-      <c r="B132" s="14"/>
-      <c r="C132" s="15"/>
-      <c r="E132" s="14"/>
-      <c r="F132" s="14"/>
-      <c r="G132" s="14"/>
+      <c r="A132" s="16"/>
+      <c r="B132" s="16"/>
+      <c r="C132" s="17"/>
+      <c r="F132" s="16"/>
+      <c r="G132" s="16"/>
+      <c r="H132" s="16"/>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="A133" s="14"/>
-      <c r="B133" s="14"/>
-      <c r="C133" s="15"/>
-      <c r="E133" s="14"/>
-      <c r="F133" s="14"/>
-      <c r="G133" s="14"/>
+      <c r="A133" s="16"/>
+      <c r="B133" s="16"/>
+      <c r="C133" s="17"/>
+      <c r="F133" s="16"/>
+      <c r="G133" s="16"/>
+      <c r="H133" s="16"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="A134" s="14"/>
-      <c r="B134" s="14"/>
-      <c r="C134" s="15"/>
-      <c r="E134" s="14"/>
-      <c r="F134" s="14"/>
-      <c r="G134" s="14"/>
+      <c r="A134" s="16"/>
+      <c r="B134" s="16"/>
+      <c r="C134" s="17"/>
+      <c r="F134" s="16"/>
+      <c r="G134" s="16"/>
+      <c r="H134" s="16"/>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="A135" s="14"/>
-      <c r="B135" s="14"/>
-      <c r="C135" s="15"/>
-      <c r="E135" s="14"/>
-      <c r="F135" s="14"/>
-      <c r="G135" s="14"/>
+      <c r="A135" s="16"/>
+      <c r="B135" s="16"/>
+      <c r="C135" s="17"/>
+      <c r="F135" s="16"/>
+      <c r="G135" s="16"/>
+      <c r="H135" s="16"/>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="A136" s="14"/>
-      <c r="B136" s="14"/>
-      <c r="C136" s="15"/>
-      <c r="E136" s="14"/>
-      <c r="F136" s="14"/>
-      <c r="G136" s="14"/>
+      <c r="A136" s="16"/>
+      <c r="B136" s="16"/>
+      <c r="C136" s="17"/>
+      <c r="F136" s="16"/>
+      <c r="G136" s="16"/>
+      <c r="H136" s="16"/>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="A137" s="14"/>
-      <c r="B137" s="14"/>
-      <c r="C137" s="15"/>
-      <c r="E137" s="14"/>
-      <c r="F137" s="14"/>
-      <c r="G137" s="14"/>
+      <c r="A137" s="16"/>
+      <c r="B137" s="16"/>
+      <c r="C137" s="17"/>
+      <c r="F137" s="16"/>
+      <c r="G137" s="16"/>
+      <c r="H137" s="16"/>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="A138" s="14"/>
-      <c r="B138" s="14"/>
-      <c r="C138" s="15"/>
-      <c r="E138" s="14"/>
-      <c r="F138" s="14"/>
-      <c r="G138" s="14"/>
+      <c r="A138" s="16"/>
+      <c r="B138" s="16"/>
+      <c r="C138" s="17"/>
+      <c r="F138" s="16"/>
+      <c r="G138" s="16"/>
+      <c r="H138" s="16"/>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="A139" s="14"/>
-      <c r="B139" s="14"/>
-      <c r="C139" s="15"/>
-      <c r="E139" s="14"/>
-      <c r="F139" s="14"/>
-      <c r="G139" s="14"/>
+      <c r="A139" s="16"/>
+      <c r="B139" s="16"/>
+      <c r="C139" s="17"/>
+      <c r="F139" s="16"/>
+      <c r="G139" s="16"/>
+      <c r="H139" s="16"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="A140" s="14"/>
-      <c r="B140" s="14"/>
-      <c r="C140" s="15"/>
-      <c r="E140" s="14"/>
-      <c r="F140" s="14"/>
-      <c r="G140" s="14"/>
+      <c r="A140" s="16"/>
+      <c r="B140" s="16"/>
+      <c r="C140" s="17"/>
+      <c r="F140" s="16"/>
+      <c r="G140" s="16"/>
+      <c r="H140" s="16"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="A141" s="14"/>
-      <c r="B141" s="14"/>
-      <c r="C141" s="15"/>
-      <c r="E141" s="14"/>
-      <c r="F141" s="14"/>
-      <c r="G141" s="14"/>
+      <c r="A141" s="16"/>
+      <c r="B141" s="16"/>
+      <c r="C141" s="17"/>
+      <c r="F141" s="16"/>
+      <c r="G141" s="16"/>
+      <c r="H141" s="16"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="A142" s="14"/>
-      <c r="B142" s="14"/>
-      <c r="C142" s="15"/>
-      <c r="E142" s="14"/>
-      <c r="F142" s="14"/>
-      <c r="G142" s="14"/>
+      <c r="A142" s="16"/>
+      <c r="B142" s="16"/>
+      <c r="C142" s="17"/>
+      <c r="F142" s="16"/>
+      <c r="G142" s="16"/>
+      <c r="H142" s="16"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="A143" s="14"/>
-      <c r="B143" s="14"/>
-      <c r="C143" s="15"/>
-      <c r="E143" s="14"/>
-      <c r="F143" s="14"/>
-      <c r="G143" s="14"/>
+      <c r="A143" s="16"/>
+      <c r="B143" s="16"/>
+      <c r="C143" s="17"/>
+      <c r="F143" s="16"/>
+      <c r="G143" s="16"/>
+      <c r="H143" s="16"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="C144" s="16"/>
+      <c r="C144" s="18"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="C145" s="17"/>
+      <c r="C145" s="19"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="C146" s="17"/>
+      <c r="C146" s="19"/>
     </row>
     <row r="147" ht="15.75" customHeight="1"/>
     <row r="148" ht="15.75" customHeight="1"/>

</xml_diff>